<commit_message>
feat: se agregó las traducciones del chivo de los risk cutoffs
</commit_message>
<xml_diff>
--- a/src/R/cut_offs_excel/cut_offs_download_ENG.xlsx
+++ b/src/R/cut_offs_excel/cut_offs_download_ENG.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/R/cut_offs_excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://paho-my.sharepoint.com/personal/caine_paho_org/Documents/WDC/Polio/2023/AR municipal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586E8CA6-1AD8-DE4C-947B-D763A0F2E213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="8_{01CF9D2D-9E2C-46D0-9867-3B7D0CE8DD2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99BED37E-DACD-4F69-A9A0-2A472FD1965A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="27740" windowHeight="16880" xr2:uid="{4197A8B5-0EC7-4519-934B-4E3E0FF6AD5B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="1" xr2:uid="{4197A8B5-0EC7-4519-934B-4E3E0FF6AD5B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Punteos de riesgo" sheetId="2" r:id="rId1"/>
+    <sheet name="Puntos" sheetId="2" r:id="rId1"/>
     <sheet name="Límites de categorías de riesgo" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -37,22 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="70">
-  <si>
-    <t>&gt;100000 o con &lt;100000 pero que si haya tenido casos de PFA</t>
-  </si>
-  <si>
-    <t>&lt;100000 que no haya tenido casos de PFA</t>
-  </si>
-  <si>
-    <t>Inmunidad</t>
-  </si>
-  <si>
-    <t>Máximo puntaje</t>
-  </si>
-  <si>
-    <t>Muy alto</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="76">
   <si>
     <t>&gt;=33</t>
   </si>
@@ -60,36 +45,24 @@
     <t>&gt;=41</t>
   </si>
   <si>
-    <t>Alto</t>
-  </si>
-  <si>
     <t>26-32</t>
   </si>
   <si>
     <t>33-40</t>
   </si>
   <si>
-    <t>Medio</t>
-  </si>
-  <si>
     <t>20-25</t>
   </si>
   <si>
     <t>25-32</t>
   </si>
   <si>
-    <t>Bajo</t>
-  </si>
-  <si>
     <t>&lt;=19</t>
   </si>
   <si>
     <t>&lt;=24</t>
   </si>
   <si>
-    <t>Vigilancia</t>
-  </si>
-  <si>
     <t>&gt;=23</t>
   </si>
   <si>
@@ -102,15 +75,6 @@
     <t>&lt;=12</t>
   </si>
   <si>
-    <t>Determinantes</t>
-  </si>
-  <si>
-    <t>No aplica</t>
-  </si>
-  <si>
-    <t>Casos y brotes de EPV</t>
-  </si>
-  <si>
     <t>&gt;=4</t>
   </si>
   <si>
@@ -129,19 +93,6 @@
     <t>&lt;=34</t>
   </si>
   <si>
-    <t>Análisis de Riesgo de Polio 2023
-País</t>
-  </si>
-  <si>
-    <t>Para municipios con &gt;100000 menores de 15 años o que hayan tenido casos de PFA en el 2022</t>
-  </si>
-  <si>
-    <t>Para municipios con &lt;100000 menores de 15 años y que no hayan tenido casos de PFA en el 2022</t>
-  </si>
-  <si>
-    <t>Cobertura Administrativa</t>
-  </si>
-  <si>
     <t>&lt;80%</t>
   </si>
   <si>
@@ -157,14 +108,104 @@
     <t>&gt;100</t>
   </si>
   <si>
-    <t>Total para los 5 años</t>
-  </si>
-  <si>
-    <t>Cobertura con IPV2</t>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>&lt; 80%</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">¿Si el país llevó a cabo una campaña de vacunación contra la polio en 2019-2023, se alcanzó una cobertura </t>
+      <t>&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>80%</t>
+    </r>
+  </si>
+  <si>
+    <t>&lt;1</t>
+  </si>
+  <si>
+    <r>
+      <t>&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <t>&lt;90%</t>
+  </si>
+  <si>
+    <r>
+      <t>&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>90%</t>
+    </r>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Polio Risk Assessment</t>
+  </si>
+  <si>
+    <t>For districts with &gt;100,000 under 15 years population and districts with &lt;100,000 that reported AFP cases during the evaluated period</t>
+  </si>
+  <si>
+    <t>Immunity</t>
+  </si>
+  <si>
+    <t>Surveillance</t>
+  </si>
+  <si>
+    <t>Determinants</t>
+  </si>
+  <si>
+    <t>Administrative coverage</t>
+  </si>
+  <si>
+    <t>IPV2 coverage</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If the country conducted a polio campaign in 2018-2022, coverage </t>
     </r>
     <r>
       <rPr>
@@ -185,29 +226,46 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>95% en el municipio?</t>
+      <t xml:space="preserve">95% was achieved in the district </t>
     </r>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Si</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>% de unidades notificadoras que enviaron información en todas las semanas durante el periodo evaluado (2023)</t>
-  </si>
-  <si>
-    <t>&lt; 80%</t>
+    <t>% of reporting units that submitted information in all weeks during the evaluated period (2022)</t>
+  </si>
+  <si>
+    <t>AFP rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% of AFP cases that were timely notified (14 days after onset of paralysis) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AFP cases investigated in less than 48 hours </t>
+  </si>
+  <si>
+    <t>AFP cases with adequate stool sample</t>
+  </si>
+  <si>
+    <t>AFP cases with  follow-up at 60 days</t>
+  </si>
+  <si>
+    <t>People using at least basic drinking water services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">People using at least basic sanitation services </t>
   </si>
   <si>
     <r>
+      <t xml:space="preserve">If the country conducted a polio campaign in the last 5 years, coverage </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>&gt;</t>
     </r>
     <r>
@@ -218,95 +276,77 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>80%</t>
+      <t xml:space="preserve">95% was achieved in the district </t>
     </r>
   </si>
   <si>
-    <t>No cuenta con unidades notificadoras</t>
-  </si>
-  <si>
-    <t>Tasa PFA</t>
-  </si>
-  <si>
-    <t>&lt;1</t>
-  </si>
-  <si>
-    <r>
-      <t>&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1</t>
-    </r>
-  </si>
-  <si>
-    <t>Búsquedas activas institucionales en al menos un establecimeinto de salud del municipio</t>
-  </si>
-  <si>
-    <t>Casos de PFA con notificación oportuna (antes de 14 días desde el inicio de la parálisis)</t>
-  </si>
-  <si>
-    <t>Porcentaje de la población con acceso a servicios básicos de agua</t>
-  </si>
-  <si>
-    <t>&lt;90%</t>
-  </si>
-  <si>
-    <r>
-      <t>&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>90%</t>
-    </r>
-  </si>
-  <si>
-    <t>Casos de PFA investigados en menos de 48 horas</t>
-  </si>
-  <si>
-    <t>Porcentaje de la población con acceso a servicios básicos de higiene</t>
-  </si>
-  <si>
-    <t>Casos de PFA con muestra adecuada de heces</t>
-  </si>
-  <si>
-    <t>Casos de PFA con seguimiento a los 60 días</t>
-  </si>
-  <si>
-    <t>Para todos los municipios</t>
-  </si>
-  <si>
-    <t>Presencia de eventos o brotes de polio o casos de sarampión, rubéola, difteria, fiebre amarilla y/o tétanos neonatal en los últimos 5 años</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>FA</t>
-  </si>
-  <si>
-    <t>TN</t>
+    <t>% of reporting units that submitted information in all weeks during the evaluated period</t>
+  </si>
+  <si>
+    <t>For all districts</t>
+  </si>
+  <si>
+    <t>VPD outbreaks and cases for all districts</t>
+  </si>
+  <si>
+    <t>Presence of measles, rubella, diphtheria or yellow fever outbreaks  and/or cases of neonatal tetanus in the last 5 years</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>YF</t>
+  </si>
+  <si>
+    <t>NT</t>
+  </si>
+  <si>
+    <t>For districts with &lt;100,000 under 15 years population that have not reported AFP cases during the evaluation period</t>
+  </si>
+  <si>
+    <t>Institutional active search conducted in at least one health establishment in the district</t>
+  </si>
+  <si>
+    <t xml:space="preserve">People using at least basic drinking water services </t>
+  </si>
+  <si>
+    <t>Total for all 5 years</t>
+  </si>
+  <si>
+    <t>No reporting units</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>Risk category</t>
+  </si>
+  <si>
+    <t>&gt;100000 or &lt;100000 but that had AFP cases</t>
+  </si>
+  <si>
+    <t>&lt;100000 that did not have AFP cases</t>
+  </si>
+  <si>
+    <t>VPD outbreaks and cases</t>
+  </si>
+  <si>
+    <t>Maximum score</t>
+  </si>
+  <si>
+    <t>Very high</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Low </t>
+  </si>
+  <si>
+    <t>Non applicable</t>
   </si>
 </sst>
 </file>
@@ -417,7 +457,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -763,11 +803,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -864,79 +945,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -948,9 +960,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -976,12 +985,106 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -991,31 +1094,26 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1054,30 +1152,28 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>108857</xdr:colOff>
+      <xdr:colOff>25400</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>43542</xdr:rowOff>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>784745</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>159655</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1145872</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>101085</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="logo ops - En-Comunicación">
+        <xdr:cNvPr id="3" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41CF4165-01FA-8444-90F7-9EB7E9CAA131}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D202D89-5D71-4DBA-836F-A36B9167682A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
+        <xdr:cNvPicPr/>
       </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
+      <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
@@ -1085,27 +1181,18 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect t="33126" b="25421"/>
-        <a:stretch/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="108857" y="43542"/>
-          <a:ext cx="2326888" cy="878113"/>
+          <a:off x="25400" y="158750"/>
+          <a:ext cx="2212672" cy="863085"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1114,9 +1201,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1154,7 +1241,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1260,7 +1347,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1402,7 +1489,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1412,155 +1499,163 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDE8A0D5-6450-1343-B741-30105C505B91}">
   <dimension ref="A1:U59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15:Q15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.6328125" customWidth="1"/>
+    <col min="2" max="2" width="22.08984375" customWidth="1"/>
+    <col min="8" max="8" width="19.81640625" customWidth="1"/>
+    <col min="12" max="12" width="14.1796875" customWidth="1"/>
+    <col min="13" max="13" width="22.54296875" customWidth="1"/>
+    <col min="19" max="19" width="18.90625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A1" s="54" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" s="54"/>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="54"/>
-      <c r="S2" s="54"/>
-      <c r="T2" s="54"/>
-      <c r="U2" s="54"/>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A3" s="54"/>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="54"/>
-      <c r="O3" s="54"/>
-      <c r="P3" s="54"/>
-      <c r="Q3" s="54"/>
-      <c r="R3" s="54"/>
-      <c r="S3" s="54"/>
-      <c r="T3" s="54"/>
-      <c r="U3" s="54"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A4" s="54"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="54"/>
-      <c r="L4" s="54"/>
-      <c r="M4" s="54"/>
-      <c r="N4" s="54"/>
-      <c r="O4" s="54"/>
-      <c r="P4" s="54"/>
-      <c r="Q4" s="54"/>
-      <c r="R4" s="54"/>
-      <c r="S4" s="54"/>
-      <c r="T4" s="54"/>
-      <c r="U4" s="54"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A5" s="54"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54"/>
-      <c r="I5" s="54"/>
-      <c r="J5" s="54"/>
-      <c r="K5" s="54"/>
-      <c r="L5" s="54"/>
-      <c r="M5" s="54"/>
-      <c r="N5" s="54"/>
-      <c r="O5" s="54"/>
-      <c r="P5" s="54"/>
-      <c r="Q5" s="54"/>
-      <c r="R5" s="54"/>
-      <c r="S5" s="54"/>
-      <c r="T5" s="54"/>
-      <c r="U5" s="54"/>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A6" s="54"/>
-      <c r="B6" s="54"/>
-      <c r="C6" s="54"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="54"/>
-      <c r="K6" s="54"/>
-      <c r="L6" s="54"/>
-      <c r="M6" s="54"/>
-      <c r="N6" s="54"/>
-      <c r="O6" s="54"/>
-      <c r="P6" s="54"/>
-      <c r="Q6" s="54"/>
-      <c r="R6" s="54"/>
-      <c r="S6" s="54"/>
-      <c r="T6" s="54"/>
-      <c r="U6" s="54"/>
-    </row>
-    <row r="7" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A1" s="63" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="63"/>
+      <c r="Q1" s="63"/>
+      <c r="R1" s="63"/>
+      <c r="S1" s="63"/>
+      <c r="T1" s="63"/>
+      <c r="U1" s="63"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A2" s="63"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="63"/>
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="63"/>
+      <c r="S2" s="63"/>
+      <c r="T2" s="63"/>
+      <c r="U2" s="63"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A3" s="63"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="63"/>
+      <c r="N3" s="63"/>
+      <c r="O3" s="63"/>
+      <c r="P3" s="63"/>
+      <c r="Q3" s="63"/>
+      <c r="R3" s="63"/>
+      <c r="S3" s="63"/>
+      <c r="T3" s="63"/>
+      <c r="U3" s="63"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A4" s="63"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="63"/>
+      <c r="K4" s="63"/>
+      <c r="L4" s="63"/>
+      <c r="M4" s="63"/>
+      <c r="N4" s="63"/>
+      <c r="O4" s="63"/>
+      <c r="P4" s="63"/>
+      <c r="Q4" s="63"/>
+      <c r="R4" s="63"/>
+      <c r="S4" s="63"/>
+      <c r="T4" s="63"/>
+      <c r="U4" s="63"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A5" s="63"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="63"/>
+      <c r="K5" s="63"/>
+      <c r="L5" s="63"/>
+      <c r="M5" s="63"/>
+      <c r="N5" s="63"/>
+      <c r="O5" s="63"/>
+      <c r="P5" s="63"/>
+      <c r="Q5" s="63"/>
+      <c r="R5" s="63"/>
+      <c r="S5" s="63"/>
+      <c r="T5" s="63"/>
+      <c r="U5" s="63"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A6" s="63"/>
+      <c r="B6" s="63"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="63"/>
+      <c r="L6" s="63"/>
+      <c r="M6" s="63"/>
+      <c r="N6" s="63"/>
+      <c r="O6" s="63"/>
+      <c r="P6" s="63"/>
+      <c r="Q6" s="63"/>
+      <c r="R6" s="63"/>
+      <c r="S6" s="63"/>
+      <c r="T6" s="63"/>
+      <c r="U6" s="63"/>
+    </row>
+    <row r="7" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -1573,7 +1668,7 @@
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
       <c r="L7" s="4" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
@@ -1584,72 +1679,72 @@
       <c r="S7" s="5"/>
       <c r="T7" s="5"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A8" s="41" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="47" t="s">
-        <v>33</v>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A8" s="64" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="66" t="s">
+        <v>41</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="G8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K8" s="5"/>
+      <c r="L8" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="H8" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="J8" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="K8" s="5"/>
-      <c r="L8" s="41" t="s">
-        <v>2</v>
-      </c>
-      <c r="M8" s="47" t="s">
-        <v>33</v>
+      <c r="M8" s="92" t="s">
+        <v>41</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="P8" s="7" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="Q8" s="8" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="R8" s="7" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="S8" s="7" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="T8" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="U8" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="42"/>
-      <c r="B9" s="44"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="65"/>
+      <c r="B9" s="67"/>
       <c r="C9" s="11">
         <v>8</v>
       </c>
@@ -1678,8 +1773,8 @@
         <v>100</v>
       </c>
       <c r="K9" s="5"/>
-      <c r="L9" s="42"/>
-      <c r="M9" s="44"/>
+      <c r="L9" s="65"/>
+      <c r="M9" s="93"/>
       <c r="N9" s="11">
         <v>10</v>
       </c>
@@ -1708,54 +1803,54 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A10" s="42"/>
-      <c r="B10" s="44" t="s">
-        <v>40</v>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A10" s="65"/>
+      <c r="B10" s="67" t="s">
+        <v>42</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="I10" s="17"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
-      <c r="L10" s="42"/>
-      <c r="M10" s="44" t="s">
-        <v>40</v>
+      <c r="L10" s="65"/>
+      <c r="M10" s="93" t="s">
+        <v>42</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="P10" s="15" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="Q10" s="16" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="R10" s="15" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="T10" s="17"/>
       <c r="U10" s="5"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A11" s="42"/>
-      <c r="B11" s="44"/>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A11" s="65"/>
+      <c r="B11" s="67"/>
       <c r="C11" s="11">
         <v>8</v>
       </c>
@@ -1774,8 +1869,8 @@
       <c r="I11" s="17"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
-      <c r="L11" s="42"/>
-      <c r="M11" s="44"/>
+      <c r="L11" s="65"/>
+      <c r="M11" s="93"/>
       <c r="N11" s="11">
         <v>10</v>
       </c>
@@ -1794,46 +1889,46 @@
       <c r="T11" s="17"/>
       <c r="U11" s="5"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A12" s="42"/>
-      <c r="B12" s="44" t="s">
-        <v>41</v>
+    <row r="12" spans="1:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="65"/>
+      <c r="B12" s="67" t="s">
+        <v>52</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="F12" s="19"/>
       <c r="G12" s="19"/>
       <c r="I12" s="17"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
-      <c r="L12" s="42"/>
-      <c r="M12" s="44" t="s">
-        <v>41</v>
+      <c r="L12" s="65"/>
+      <c r="M12" s="67" t="s">
+        <v>43</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="Q12" s="19"/>
       <c r="R12" s="19"/>
       <c r="T12" s="17"/>
       <c r="U12" s="5"/>
     </row>
-    <row r="13" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="42"/>
-      <c r="B13" s="53"/>
+    <row r="13" spans="1:21" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="65"/>
+      <c r="B13" s="69"/>
       <c r="C13" s="20">
         <v>6</v>
       </c>
@@ -1848,8 +1943,8 @@
       <c r="I13" s="17"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
-      <c r="L13" s="43"/>
-      <c r="M13" s="45"/>
+      <c r="L13" s="65"/>
+      <c r="M13" s="69"/>
       <c r="N13" s="11">
         <v>8</v>
       </c>
@@ -1864,23 +1959,23 @@
       <c r="T13" s="17"/>
       <c r="U13" s="5"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A14" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="48" t="s">
-        <v>46</v>
+    <row r="14" spans="1:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="64" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="73" t="s">
+        <v>53</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" s="50" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" s="50"/>
+        <v>28</v>
+      </c>
+      <c r="E14" s="71" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" s="71"/>
       <c r="G14" s="22"/>
       <c r="H14" s="23"/>
       <c r="I14" s="24">
@@ -1889,22 +1984,22 @@
       </c>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
-      <c r="L14" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="M14" s="51" t="s">
-        <v>46</v>
+      <c r="L14" s="78" t="s">
+        <v>39</v>
+      </c>
+      <c r="M14" s="73" t="s">
+        <v>44</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="O14" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="P14" s="50" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q14" s="50"/>
+        <v>28</v>
+      </c>
+      <c r="P14" s="71" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q14" s="71"/>
       <c r="R14" s="22"/>
       <c r="S14" s="23"/>
       <c r="T14" s="24">
@@ -1913,71 +2008,71 @@
       </c>
       <c r="U14" s="5"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A15" s="42"/>
-      <c r="B15" s="49"/>
+    <row r="15" spans="1:21" ht="71.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="65"/>
+      <c r="B15" s="74"/>
       <c r="C15" s="25">
         <v>8</v>
       </c>
       <c r="D15" s="25">
         <v>0</v>
       </c>
-      <c r="E15" s="52">
+      <c r="E15" s="72">
         <v>8</v>
       </c>
-      <c r="F15" s="52"/>
+      <c r="F15" s="72"/>
       <c r="G15" s="26"/>
       <c r="I15" s="17"/>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
-      <c r="L15" s="42"/>
-      <c r="M15" s="49"/>
+      <c r="L15" s="79"/>
+      <c r="M15" s="74"/>
       <c r="N15" s="25">
         <v>8</v>
       </c>
       <c r="O15" s="25">
         <v>0</v>
       </c>
-      <c r="P15" s="52">
+      <c r="P15" s="72">
         <v>8</v>
       </c>
-      <c r="Q15" s="52"/>
+      <c r="Q15" s="72"/>
       <c r="R15" s="26"/>
       <c r="T15" s="17"/>
       <c r="U15" s="5"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A16" s="42"/>
-      <c r="B16" s="44" t="s">
-        <v>50</v>
+    <row r="16" spans="1:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="65"/>
+      <c r="B16" s="67" t="s">
+        <v>45</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="D16" s="27" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="E16" s="19"/>
       <c r="I16" s="17"/>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
-      <c r="L16" s="42"/>
-      <c r="M16" s="44" t="s">
-        <v>53</v>
+      <c r="L16" s="79"/>
+      <c r="M16" s="67" t="s">
+        <v>61</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="P16" s="19"/>
       <c r="T16" s="17"/>
       <c r="U16" s="5"/>
     </row>
-    <row r="17" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="42"/>
-      <c r="B17" s="44"/>
+    <row r="17" spans="1:21" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="65"/>
+      <c r="B17" s="67"/>
       <c r="C17" s="11">
         <v>8</v>
       </c>
@@ -1988,8 +2083,8 @@
       <c r="I17" s="17"/>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
-      <c r="L17" s="42"/>
-      <c r="M17" s="53"/>
+      <c r="L17" s="80"/>
+      <c r="M17" s="70"/>
       <c r="N17" s="20">
         <v>12</v>
       </c>
@@ -2000,32 +2095,32 @@
       <c r="T17" s="17"/>
       <c r="U17" s="5"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A18" s="42"/>
-      <c r="B18" s="44" t="s">
-        <v>54</v>
+    <row r="18" spans="1:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="65"/>
+      <c r="B18" s="67" t="s">
+        <v>46</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="D18" s="28" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="E18" s="19"/>
       <c r="I18" s="17"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
-      <c r="L18" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="M18" s="47" t="s">
-        <v>55</v>
+      <c r="L18" s="94" t="s">
+        <v>40</v>
+      </c>
+      <c r="M18" s="95" t="s">
+        <v>62</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="O18" s="27" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="P18" s="23"/>
       <c r="Q18" s="23"/>
@@ -2037,9 +2132,9 @@
       </c>
       <c r="U18" s="5"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A19" s="42"/>
-      <c r="B19" s="44"/>
+    <row r="19" spans="1:21" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="65"/>
+      <c r="B19" s="67"/>
       <c r="C19" s="11">
         <v>5</v>
       </c>
@@ -2050,8 +2145,8 @@
       <c r="I19" s="17"/>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
-      <c r="L19" s="37"/>
-      <c r="M19" s="44"/>
+      <c r="L19" s="79"/>
+      <c r="M19" s="67"/>
       <c r="N19" s="11">
         <v>6</v>
       </c>
@@ -2061,37 +2156,37 @@
       <c r="T19" s="17"/>
       <c r="U19" s="5"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A20" s="42"/>
-      <c r="B20" s="44" t="s">
-        <v>58</v>
+    <row r="20" spans="1:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="65"/>
+      <c r="B20" s="67" t="s">
+        <v>47</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="D20" s="28" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="E20" s="19"/>
       <c r="I20" s="17"/>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
-      <c r="L20" s="37"/>
-      <c r="M20" s="44" t="s">
-        <v>59</v>
+      <c r="L20" s="79"/>
+      <c r="M20" s="67" t="s">
+        <v>51</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="O20" s="28" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="T20" s="17"/>
       <c r="U20" s="5"/>
     </row>
-    <row r="21" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="42"/>
-      <c r="B21" s="44"/>
+    <row r="21" spans="1:21" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="65"/>
+      <c r="B21" s="67"/>
       <c r="C21" s="11">
         <v>5</v>
       </c>
@@ -2102,8 +2197,8 @@
       <c r="I21" s="17"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
-      <c r="L21" s="38"/>
-      <c r="M21" s="45"/>
+      <c r="L21" s="80"/>
+      <c r="M21" s="70"/>
       <c r="N21" s="29">
         <v>6</v>
       </c>
@@ -2117,16 +2212,16 @@
       <c r="T21" s="31"/>
       <c r="U21" s="5"/>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A22" s="42"/>
-      <c r="B22" s="44" t="s">
-        <v>60</v>
+    <row r="22" spans="1:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="65"/>
+      <c r="B22" s="67" t="s">
+        <v>48</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="D22" s="28" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="E22" s="19"/>
       <c r="I22" s="17"/>
@@ -2143,9 +2238,9 @@
       <c r="T22" s="5"/>
       <c r="U22" s="5"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A23" s="42"/>
-      <c r="B23" s="44"/>
+    <row r="23" spans="1:21" ht="43" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="65"/>
+      <c r="B23" s="67"/>
       <c r="C23" s="11">
         <v>5</v>
       </c>
@@ -2167,16 +2262,16 @@
       <c r="T23" s="5"/>
       <c r="U23" s="5"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A24" s="42"/>
-      <c r="B24" s="44" t="s">
-        <v>61</v>
+    <row r="24" spans="1:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="65"/>
+      <c r="B24" s="67" t="s">
+        <v>49</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="D24" s="28" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="E24" s="19"/>
       <c r="I24" s="17"/>
@@ -2193,9 +2288,9 @@
       <c r="T24" s="5"/>
       <c r="U24" s="5"/>
     </row>
-    <row r="25" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="43"/>
-      <c r="B25" s="45"/>
+    <row r="25" spans="1:21" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="68"/>
+      <c r="B25" s="70"/>
       <c r="C25" s="29">
         <v>5</v>
       </c>
@@ -2210,7 +2305,7 @@
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
-      <c r="M25" s="46"/>
+      <c r="M25" s="77"/>
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
       <c r="P25" s="5"/>
@@ -2220,18 +2315,18 @@
       <c r="T25" s="5"/>
       <c r="U25" s="5"/>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A26" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" s="47" t="s">
-        <v>55</v>
+    <row r="26" spans="1:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="78" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="66" t="s">
+        <v>50</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="E26" s="23"/>
       <c r="F26" s="23"/>
@@ -2244,7 +2339,7 @@
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
-      <c r="M26" s="46"/>
+      <c r="M26" s="77"/>
       <c r="N26" s="5"/>
       <c r="O26" s="5"/>
       <c r="P26" s="5"/>
@@ -2254,9 +2349,9 @@
       <c r="T26" s="5"/>
       <c r="U26" s="5"/>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A27" s="37"/>
-      <c r="B27" s="44"/>
+    <row r="27" spans="1:21" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="79"/>
+      <c r="B27" s="67"/>
       <c r="C27" s="11">
         <v>5</v>
       </c>
@@ -2277,16 +2372,16 @@
       <c r="T27" s="5"/>
       <c r="U27" s="5"/>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A28" s="37"/>
-      <c r="B28" s="44" t="s">
-        <v>59</v>
+    <row r="28" spans="1:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="79"/>
+      <c r="B28" s="67" t="s">
+        <v>51</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D28" s="28" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="I28" s="17"/>
       <c r="J28" s="5"/>
@@ -2302,9 +2397,9 @@
       <c r="T28" s="5"/>
       <c r="U28" s="5"/>
     </row>
-    <row r="29" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="38"/>
-      <c r="B29" s="45"/>
+    <row r="29" spans="1:21" ht="51.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="80"/>
+      <c r="B29" s="70"/>
       <c r="C29" s="29">
         <v>5</v>
       </c>
@@ -2329,7 +2424,7 @@
       <c r="T29" s="5"/>
       <c r="U29" s="5"/>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:21" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -2352,9 +2447,9 @@
       <c r="T30" s="5"/>
       <c r="U30" s="5"/>
     </row>
-    <row r="31" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="4" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -2377,30 +2472,30 @@
       <c r="T31" s="5"/>
       <c r="U31" s="5"/>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A32" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="B32" s="47" t="s">
-        <v>63</v>
+    <row r="32" spans="1:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="75" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" s="66" t="s">
+        <v>56</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>66</v>
+        <v>34</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="I32" s="6"/>
       <c r="J32" s="5"/>
@@ -2416,9 +2511,9 @@
       <c r="T32" s="5"/>
       <c r="U32" s="5"/>
     </row>
-    <row r="33" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="40"/>
-      <c r="B33" s="45"/>
+    <row r="33" spans="1:21" ht="72.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="76"/>
+      <c r="B33" s="70"/>
       <c r="C33" s="33">
         <v>4</v>
       </c>
@@ -2440,7 +2535,7 @@
       <c r="I33" s="6"/>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
-      <c r="L33" s="46"/>
+      <c r="L33" s="77"/>
       <c r="M33" s="5"/>
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
@@ -2451,162 +2546,160 @@
       <c r="T33" s="5"/>
       <c r="U33" s="5"/>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.35">
       <c r="I34" s="35"/>
-      <c r="L34" s="46"/>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A35" s="86"/>
-      <c r="B35" s="86"/>
-      <c r="C35" s="87"/>
-      <c r="D35" s="87"/>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A36" s="91"/>
-      <c r="B36" s="86"/>
-      <c r="C36" s="88"/>
-      <c r="D36" s="88"/>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A37" s="91"/>
-      <c r="B37" s="86"/>
-      <c r="C37" s="88"/>
-      <c r="D37" s="88"/>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A38" s="91"/>
-      <c r="B38" s="86"/>
-      <c r="C38" s="88"/>
-      <c r="D38" s="88"/>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A39" s="91"/>
-      <c r="B39" s="86"/>
-      <c r="C39" s="88"/>
-      <c r="D39" s="88"/>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A40" s="91"/>
-      <c r="B40" s="86"/>
-      <c r="C40" s="88"/>
-      <c r="D40" s="88"/>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A41" s="91"/>
-      <c r="B41" s="86"/>
-      <c r="C41" s="88"/>
-      <c r="D41" s="88"/>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A42" s="91"/>
-      <c r="B42" s="86"/>
-      <c r="C42" s="88"/>
-      <c r="D42" s="88"/>
-    </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A43" s="91"/>
-      <c r="B43" s="86"/>
-      <c r="C43" s="88"/>
-      <c r="D43" s="89"/>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A44" s="91"/>
-      <c r="B44" s="86"/>
-      <c r="C44" s="88"/>
-      <c r="D44" s="89"/>
-    </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A45" s="91"/>
-      <c r="B45" s="86"/>
-      <c r="C45" s="88"/>
-      <c r="D45" s="88"/>
-    </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A46" s="91"/>
-      <c r="B46" s="86"/>
-      <c r="C46" s="90"/>
-      <c r="D46" s="88"/>
-    </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A47" s="91"/>
-      <c r="B47" s="86"/>
-      <c r="C47" s="88"/>
-      <c r="D47" s="88"/>
-    </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A48" s="91"/>
-      <c r="B48" s="86"/>
-      <c r="C48" s="90"/>
-      <c r="D48" s="90"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="91"/>
-      <c r="B49" s="86"/>
-      <c r="C49" s="90"/>
-      <c r="D49" s="90"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="91"/>
-      <c r="B50" s="86"/>
-      <c r="C50" s="90"/>
-      <c r="D50" s="90"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="92"/>
-      <c r="B51" s="86"/>
-      <c r="C51" s="90"/>
-      <c r="D51" s="90"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="92"/>
-      <c r="B52" s="86"/>
-      <c r="C52" s="88"/>
-      <c r="D52" s="88"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="92"/>
-      <c r="B53" s="86"/>
-      <c r="C53" s="90"/>
-      <c r="D53" s="90"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="92"/>
-      <c r="B54" s="86"/>
-      <c r="C54" s="90"/>
-      <c r="D54" s="90"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="92"/>
-      <c r="B55" s="86"/>
-      <c r="C55" s="90"/>
-      <c r="D55" s="90"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="91"/>
-      <c r="B56" s="86"/>
-      <c r="C56" s="90"/>
-      <c r="D56" s="90"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="91"/>
-      <c r="B57" s="86"/>
-      <c r="C57" s="90"/>
-      <c r="D57" s="90"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="91"/>
-      <c r="B58" s="86"/>
-      <c r="C58" s="90"/>
-      <c r="D58" s="90"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="91"/>
-      <c r="B59" s="86"/>
-      <c r="C59" s="90"/>
-      <c r="D59" s="90"/>
+      <c r="L34" s="77"/>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="C35" s="53"/>
+      <c r="D35" s="53"/>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A36" s="56"/>
+      <c r="C36" s="54"/>
+      <c r="D36" s="54"/>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A37" s="56"/>
+      <c r="C37" s="54"/>
+      <c r="D37" s="54"/>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A38" s="56"/>
+      <c r="C38" s="54"/>
+      <c r="D38" s="54"/>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A39" s="56"/>
+      <c r="C39" s="54"/>
+      <c r="D39" s="54"/>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A40" s="56"/>
+      <c r="C40" s="54"/>
+      <c r="D40" s="54"/>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A41" s="56"/>
+      <c r="C41" s="54"/>
+      <c r="D41" s="54"/>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A42" s="56"/>
+      <c r="C42" s="54"/>
+      <c r="D42" s="54"/>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A43" s="56"/>
+      <c r="C43" s="54"/>
+      <c r="D43" s="55"/>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A44" s="56"/>
+      <c r="C44" s="54"/>
+      <c r="D44" s="55"/>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A45" s="56"/>
+      <c r="C45" s="54"/>
+      <c r="D45" s="54"/>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A46" s="56"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="54"/>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A47" s="56"/>
+      <c r="C47" s="54"/>
+      <c r="D47" s="54"/>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A48" s="56"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="19"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A49" s="56"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="19"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A50" s="56"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A51" s="57"/>
+      <c r="C51" s="19"/>
+      <c r="D51" s="19"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A52" s="57"/>
+      <c r="C52" s="54"/>
+      <c r="D52" s="54"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A53" s="57"/>
+      <c r="C53" s="19"/>
+      <c r="D53" s="19"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A54" s="57"/>
+      <c r="C54" s="19"/>
+      <c r="D54" s="19"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A55" s="57"/>
+      <c r="C55" s="19"/>
+      <c r="D55" s="19"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A56" s="56"/>
+      <c r="C56" s="19"/>
+      <c r="D56" s="19"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57" s="56"/>
+      <c r="C57" s="19"/>
+      <c r="D57" s="19"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A58" s="56"/>
+      <c r="C58" s="19"/>
+      <c r="D58" s="19"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A59" s="56"/>
+      <c r="C59" s="19"/>
+      <c r="D59" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="L33:L34"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="L18:L21"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="M20:M21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="L14:L17"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="M16:M17"/>
     <mergeCell ref="A1:U6"/>
     <mergeCell ref="A8:A13"/>
     <mergeCell ref="B8:B9"/>
@@ -2616,30 +2709,6 @@
     <mergeCell ref="M10:M11"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="M12:M13"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="M20:M21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="L14:L17"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="L33:L34"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="L18:L21"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="M25:M26"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B28:B29"/>
   </mergeCells>
   <conditionalFormatting sqref="J9">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="notEqual">
@@ -2660,323 +2729,327 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70F1F3C2-CE97-4E8C-8744-58BD9E002719}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="35.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.453125" customWidth="1"/>
+    <col min="2" max="2" width="21.6328125" customWidth="1"/>
+    <col min="3" max="4" width="35.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="41" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="55"/>
-      <c r="B1" s="56"/>
-      <c r="C1" s="57" t="s">
+    <row r="1" spans="1:4" ht="37.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="62" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="91" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="61" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A2" s="81" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="58" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="59">
+        <v>54</v>
+      </c>
+      <c r="D2" s="60">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A3" s="82"/>
+      <c r="B3" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="57" t="s">
+      <c r="D3" s="40" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="58" t="s">
+    <row r="4" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A4" s="82"/>
+      <c r="B4" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="59" t="s">
+      <c r="D4" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="60">
-        <v>54</v>
-      </c>
-      <c r="D2" s="61">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="62"/>
-      <c r="B3" s="63" t="s">
+    </row>
+    <row r="5" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A5" s="82"/>
+      <c r="B5" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="64" t="s">
+      <c r="D5" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="65" t="s">
+    </row>
+    <row r="6" spans="1:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A6" s="83"/>
+      <c r="B6" s="43" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="44" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="62"/>
-      <c r="B4" s="66" t="s">
+      <c r="D6" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="64" t="s">
+    </row>
+    <row r="7" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="84" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="58" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="36">
+        <v>36</v>
+      </c>
+      <c r="D7" s="37">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A8" s="82"/>
+      <c r="B8" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="65" t="s">
+      <c r="D8" s="40">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A9" s="82"/>
+      <c r="B9" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="39" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="62"/>
-      <c r="B5" s="67" t="s">
+      <c r="D9" s="46">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A10" s="82"/>
+      <c r="B10" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="64" t="s">
+      <c r="D10" s="46">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A11" s="83"/>
+      <c r="B11" s="43" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="65" t="s">
+      <c r="D11" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A12" s="84" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="58" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="47">
+        <v>10</v>
+      </c>
+      <c r="D12" s="37">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="68"/>
-      <c r="B6" s="69" t="s">
+    <row r="13" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A13" s="82"/>
+      <c r="B13" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="39" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A14" s="82"/>
+      <c r="B14" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" s="48">
+        <v>10</v>
+      </c>
+      <c r="D14" s="49">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A15" s="82"/>
+      <c r="B15" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="48">
+        <v>5</v>
+      </c>
+      <c r="D15" s="49">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A16" s="83"/>
+      <c r="B16" s="43" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="50">
+        <v>0</v>
+      </c>
+      <c r="D16" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A17" s="85" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="58" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="47">
+        <v>14</v>
+      </c>
+      <c r="D17" s="52">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A18" s="86"/>
+      <c r="B18" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" s="39" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A19" s="86"/>
+      <c r="B19" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="49" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A20" s="86"/>
+      <c r="B20" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="48">
+        <v>2</v>
+      </c>
+      <c r="D20" s="49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A21" s="87"/>
+      <c r="B21" s="43" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="50">
+        <v>0</v>
+      </c>
+      <c r="D21" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A22" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="70" t="s">
+      <c r="B22" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="71" t="s">
+      <c r="D22" s="52" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A23" s="89"/>
+      <c r="B23" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="48" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A7" s="58" t="s">
+      <c r="D23" s="49" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A24" s="89"/>
+      <c r="B24" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="59" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="60">
-        <v>36</v>
-      </c>
-      <c r="D7" s="61">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A8" s="62"/>
-      <c r="B8" s="63" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="64" t="s">
+      <c r="D24" s="49" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A25" s="90"/>
+      <c r="B25" s="43" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="65">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="62"/>
-      <c r="B9" s="66" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="64" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="72">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A10" s="62"/>
-      <c r="B10" s="67" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="64" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="72">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="68"/>
-      <c r="B11" s="69" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="70" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A12" s="58" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="59" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="73">
-        <v>10</v>
-      </c>
-      <c r="D12" s="61">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A13" s="62"/>
-      <c r="B13" s="63" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="64" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="65" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A14" s="62"/>
-      <c r="B14" s="66" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="74">
-        <v>10</v>
-      </c>
-      <c r="D14" s="75">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A15" s="62"/>
-      <c r="B15" s="67" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="74">
-        <v>5</v>
-      </c>
-      <c r="D15" s="75">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="68"/>
-      <c r="B16" s="69" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="76">
-        <v>0</v>
-      </c>
-      <c r="D16" s="77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A17" s="78" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="59" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="73">
-        <v>14</v>
-      </c>
-      <c r="D17" s="79">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A18" s="80"/>
-      <c r="B18" s="63" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="64" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="65" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A19" s="80"/>
-      <c r="B19" s="66" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="74" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="75" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A20" s="80"/>
-      <c r="B20" s="67" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="74">
-        <v>2</v>
-      </c>
-      <c r="D20" s="75">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="81"/>
-      <c r="B21" s="69" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="76">
-        <v>0</v>
-      </c>
-      <c r="D21" s="77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A22" s="82" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="83" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="73" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" s="79" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A23" s="84"/>
-      <c r="B23" s="66" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="74" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23" s="75" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A24" s="84"/>
-      <c r="B24" s="67" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="74" t="s">
-        <v>28</v>
-      </c>
-      <c r="D24" s="75" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="85"/>
-      <c r="B25" s="69" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="76" t="s">
-        <v>29</v>
-      </c>
-      <c r="D25" s="77" t="s">
-        <v>29</v>
+      <c r="D25" s="51" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>